<commit_message>
update logbook en actieplan
</commit_message>
<xml_diff>
--- a/Actieplan_Python.xlsx
+++ b/Actieplan_Python.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/f020cdb928d38096/Programmeren/Odisee/LevensLang_Leren/LLL-BartBrondeel-2526/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="13_ncr:1_{482E40B1-4C12-41F6-8D36-DD9DCD6004AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{9C609046-2913-4D70-BFDB-8724F256E8AC}"/>
+  <xr:revisionPtr revIDLastSave="16" documentId="13_ncr:1_{482E40B1-4C12-41F6-8D36-DD9DCD6004AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1EDE279F-45DC-49D4-B35C-B780924A38B7}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Actieplan" sheetId="1" r:id="rId1"/>
@@ -642,7 +642,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J22"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -760,7 +760,7 @@
       <c r="H4" s="10"/>
       <c r="I4" s="10">
         <f>('Werkelijke uren'!D32)</f>
-        <v>25.75</v>
+        <v>30.5</v>
       </c>
       <c r="J4" s="10" t="s">
         <v>21</v>
@@ -835,7 +835,7 @@
       <c r="H7" s="10"/>
       <c r="I7" s="10">
         <f>('Werkelijke uren'!C103)</f>
-        <v>25.75</v>
+        <v>30.5</v>
       </c>
       <c r="J7" s="10"/>
     </row>
@@ -1146,7 +1146,7 @@
       </c>
       <c r="I22">
         <f>SUM(I7,I14,I20)</f>
-        <v>25.75</v>
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>
@@ -1163,8 +1163,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B3793691-12BB-4C09-897D-D3E0C91FA681}">
   <dimension ref="B2:D103"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="I14" sqref="I14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1277,11 +1277,17 @@
       <c r="B15">
         <v>13</v>
       </c>
+      <c r="C15">
+        <v>1.75</v>
+      </c>
     </row>
     <row r="16" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>14</v>
       </c>
+      <c r="C16">
+        <v>3</v>
+      </c>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17">
@@ -1364,7 +1370,7 @@
       </c>
       <c r="D32">
         <f>SUM(C3:C32)</f>
-        <v>25.75</v>
+        <v>30.5</v>
       </c>
     </row>
     <row r="33" spans="2:2" x14ac:dyDescent="0.25">
@@ -1731,7 +1737,7 @@
       </c>
       <c r="C103">
         <f>SUM(C3:C102)</f>
-        <v>25.75</v>
+        <v>30.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>